<commit_message>
code for venn diagrams
</commit_message>
<xml_diff>
--- a/manualFIC.xlsx
+++ b/manualFIC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruth\Desktop\MetS python Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Dev\Stats-Mets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9072CFAC-3F8C-43A1-80D4-961FD4E31F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B6CDE0-991D-48FD-98D5-7D97DFBEBA8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Merge clean" sheetId="26" r:id="rId1"/>
@@ -23,29 +23,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -1325,7 +1315,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1334,13 +1324,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.34998626667073579"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1372,16 +1356,16 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1701,17 +1685,17 @@
   <dimension ref="A1:H401"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="G275" sqref="G275"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="8.7265625" style="2"/>
-    <col min="7" max="8" width="8.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="6" width="8.7109375" style="2"/>
+    <col min="7" max="8" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1737,7 +1721,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1763,7 +1747,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1789,7 +1773,7 @@
         <v>4.4746128480094924</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1815,7 +1799,7 @@
         <v>4.1936868578849014</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1841,7 +1825,7 @@
         <v>5.295538225635477</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1867,7 +1851,7 @@
         <v>4.3151835105429424</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1893,7 +1877,7 @@
         <v>5.1075399326132134</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1919,7 +1903,7 @@
         <v>4.5667131468688638</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1945,7 +1929,7 @@
         <v>2.4901280915375832</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1971,7 +1955,7 @@
         <v>4.2631406693710465</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1997,7 +1981,7 @@
         <v>2.8869903864861763</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -2023,7 +2007,7 @@
         <v>5.2902147379081788</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -2049,7 +2033,7 @@
         <v>2.6500511648194243</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -2075,7 +2059,7 @@
         <v>4.9617754921599442</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -2101,7 +2085,7 @@
         <v>6.6211969593952364</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -2127,7 +2111,7 @@
         <v>1.6364981552279041</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -2153,7 +2137,7 @@
         <v>4.6723817363442288</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -2179,7 +2163,7 @@
         <v>3.4844663192005516</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -2205,7 +2189,7 @@
         <v>3.5397622870609715</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -2231,7 +2215,7 @@
         <v>3.4380999268941328</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -2257,7 +2241,7 @@
         <v>2.1843649277796038</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -2283,7 +2267,7 @@
         <v>13.227367762726862</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -2309,7 +2293,7 @@
         <v>5.7864967904598856</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -2335,7 +2319,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -2361,7 +2345,7 @@
         <v>6.67</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -2387,7 +2371,7 @@
         <v>8.89</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
@@ -2413,7 +2397,7 @@
         <v>5.92</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -2439,7 +2423,7 @@
         <v>5.18</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -2465,7 +2449,7 @@
         <v>5.92</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>41</v>
       </c>
@@ -2491,7 +2475,7 @@
         <v>8.15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
@@ -2517,7 +2501,7 @@
         <v>7.41</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -2543,7 +2527,7 @@
         <v>7.41</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -2562,12 +2546,12 @@
       <c r="F33" s="2">
         <v>84</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="6">
         <v>0</v>
       </c>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
@@ -2593,7 +2577,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>36</v>
       </c>
@@ -2619,7 +2603,7 @@
         <v>5.92</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -2645,7 +2629,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>34</v>
       </c>
@@ -2671,7 +2655,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>33</v>
       </c>
@@ -2697,7 +2681,7 @@
         <v>5.92</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>84</v>
       </c>
@@ -2723,7 +2707,7 @@
         <v>4.3650816034846533</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>85</v>
       </c>
@@ -2747,7 +2731,7 @@
         <v>4.2013311720346742</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>86</v>
       </c>
@@ -2773,7 +2757,7 @@
         <v>4.7811339563862925</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>87</v>
       </c>
@@ -2799,7 +2783,7 @@
         <v>5.7878238722984481</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>88</v>
       </c>
@@ -2825,7 +2809,7 @@
         <v>4.5167313692184532</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>215</v>
       </c>
@@ -2851,7 +2835,7 @@
         <v>3.6240000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>216</v>
       </c>
@@ -2877,7 +2861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>217</v>
       </c>
@@ -2903,7 +2887,7 @@
         <v>6.5655337754423506</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>218</v>
       </c>
@@ -2929,7 +2913,7 @@
         <v>7.0846777270946815</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>219</v>
       </c>
@@ -2955,7 +2939,7 @@
         <v>5.1734926854018095</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>220</v>
       </c>
@@ -2981,7 +2965,7 @@
         <v>13.453698942531672</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>221</v>
       </c>
@@ -3007,7 +2991,7 @@
         <v>10.107649351363944</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>222</v>
       </c>
@@ -3033,7 +3017,7 @@
         <v>7.8350654352911215</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>223</v>
       </c>
@@ -3059,7 +3043,7 @@
         <v>7.6704135507078268</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>224</v>
       </c>
@@ -3085,7 +3069,7 @@
         <v>8.8831175379310672</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>175</v>
       </c>
@@ -3111,7 +3095,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>176</v>
       </c>
@@ -3137,7 +3121,7 @@
         <v>7.86980638768937</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>177</v>
       </c>
@@ -3163,7 +3147,7 @@
         <v>10.735177437149275</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>178</v>
       </c>
@@ -3189,7 +3173,7 @@
         <v>10.633212664113787</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>179</v>
       </c>
@@ -3215,7 +3199,7 @@
         <v>11.722100272350445</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>180</v>
       </c>
@@ -3241,7 +3225,7 @@
         <v>7.9534635517226588</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>181</v>
       </c>
@@ -3267,7 +3251,7 @@
         <v>6.6766368617043721</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>182</v>
       </c>
@@ -3293,7 +3277,7 @@
         <v>9.2293861556727119</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>183</v>
       </c>
@@ -3319,7 +3303,7 @@
         <v>8.5679051094295655</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>184</v>
       </c>
@@ -3345,7 +3329,7 @@
         <v>6.8164208638964663</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>185</v>
       </c>
@@ -3371,7 +3355,7 @@
         <v>5.9234366642353509</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>186</v>
       </c>
@@ -3397,7 +3381,7 @@
         <v>5.3386560939449046</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>187</v>
       </c>
@@ -3423,7 +3407,7 @@
         <v>8.0616739401814694</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>188</v>
       </c>
@@ -3449,7 +3433,7 @@
         <v>3.8631108679795769</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>189</v>
       </c>
@@ -3475,7 +3459,7 @@
         <v>4.1084255531841993</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>190</v>
       </c>
@@ -3501,7 +3485,7 @@
         <v>6.6812819110138584</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>191</v>
       </c>
@@ -3527,7 +3511,7 @@
         <v>6.4460928404914117</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>192</v>
       </c>
@@ -3553,7 +3537,7 @@
         <v>9.1080105742332034</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>193</v>
       </c>
@@ -3579,7 +3563,7 @@
         <v>6.8292952242220855</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>194</v>
       </c>
@@ -3605,7 +3589,7 @@
         <v>3.7422279047338787</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>195</v>
       </c>
@@ -3631,7 +3615,7 @@
         <v>4.7836819684342862</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>196</v>
       </c>
@@ -3657,7 +3641,7 @@
         <v>4.3209610449253057</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>197</v>
       </c>
@@ -3683,7 +3667,7 @@
         <v>7.0681673111440055</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>198</v>
       </c>
@@ -3709,7 +3693,7 @@
         <v>4.5564897417195009</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>199</v>
       </c>
@@ -3735,7 +3719,7 @@
         <v>7.9208323117001216</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>200</v>
       </c>
@@ -3761,7 +3745,7 @@
         <v>7.7439153735224187</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>201</v>
       </c>
@@ -3787,7 +3771,7 @@
         <v>3.8037436318086502</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>202</v>
       </c>
@@ -3813,7 +3797,7 @@
         <v>7.3342040627794658</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>203</v>
       </c>
@@ -3839,7 +3823,7 @@
         <v>4.1514973232594308</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>204</v>
       </c>
@@ -3865,7 +3849,7 @@
         <v>6.1826829564794563</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>205</v>
       </c>
@@ -3891,7 +3875,7 @@
         <v>8.0312943777073187</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>206</v>
       </c>
@@ -3917,7 +3901,7 @@
         <v>7.1716271894327708</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>207</v>
       </c>
@@ -3943,7 +3927,7 @@
         <v>9.4111956251842876</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>208</v>
       </c>
@@ -3969,7 +3953,7 @@
         <v>5.059998816862354</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>209</v>
       </c>
@@ -3995,7 +3979,7 @@
         <v>7.8360532095157085</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>210</v>
       </c>
@@ -4021,7 +4005,7 @@
         <v>8.365003847987273</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>211</v>
       </c>
@@ -4043,7 +4027,7 @@
         <v>11.148398314067126</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>212</v>
       </c>
@@ -4069,7 +4053,7 @@
         <v>6.9599372535709616</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>213</v>
       </c>
@@ -4095,7 +4079,7 @@
         <v>7.8812717639937082</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>214</v>
       </c>
@@ -4121,7 +4105,7 @@
         <v>8.6640868021738484</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>225</v>
       </c>
@@ -4147,7 +4131,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>226</v>
       </c>
@@ -4173,7 +4157,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>228</v>
       </c>
@@ -4199,7 +4183,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>229</v>
       </c>
@@ -4225,7 +4209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>230</v>
       </c>
@@ -4249,7 +4233,7 @@
       </c>
       <c r="H98" s="3"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>231</v>
       </c>
@@ -4275,7 +4259,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>232</v>
       </c>
@@ -4301,7 +4285,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>233</v>
       </c>
@@ -4327,7 +4311,7 @@
         <v>6.37</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>234</v>
       </c>
@@ -4353,7 +4337,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>235</v>
       </c>
@@ -4379,7 +4363,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>236</v>
       </c>
@@ -4405,7 +4389,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>237</v>
       </c>
@@ -4431,7 +4415,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>238</v>
       </c>
@@ -4457,7 +4441,7 @@
         <v>6.22</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>239</v>
       </c>
@@ -4483,7 +4467,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>240</v>
       </c>
@@ -4509,7 +4493,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>241</v>
       </c>
@@ -4535,7 +4519,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>242</v>
       </c>
@@ -4561,7 +4545,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>243</v>
       </c>
@@ -4587,7 +4571,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>244</v>
       </c>
@@ -4613,7 +4597,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>245</v>
       </c>
@@ -4639,7 +4623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>246</v>
       </c>
@@ -4665,7 +4649,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>247</v>
       </c>
@@ -4691,7 +4675,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>248</v>
       </c>
@@ -4717,7 +4701,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>249</v>
       </c>
@@ -4743,7 +4727,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>250</v>
       </c>
@@ -4769,7 +4753,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>251</v>
       </c>
@@ -4795,7 +4779,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>252</v>
       </c>
@@ -4821,7 +4805,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>253</v>
       </c>
@@ -4837,13 +4821,13 @@
       <c r="E121" s="3">
         <v>0.93442622950819676</v>
       </c>
-      <c r="F121" s="5"/>
-      <c r="G121" s="6"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="5"/>
       <c r="H121" s="3">
         <v>10.81</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>254</v>
       </c>
@@ -4859,13 +4843,13 @@
       <c r="E122" s="3">
         <v>0.98039215686274506</v>
       </c>
-      <c r="F122" s="5"/>
-      <c r="G122" s="6"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="5"/>
       <c r="H122" s="3">
         <v>11.04</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>42</v>
       </c>
@@ -4891,7 +4875,7 @@
         <v>3.2782805583176806</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>43</v>
       </c>
@@ -4917,7 +4901,7 @@
         <v>6.44</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>44</v>
       </c>
@@ -4943,7 +4927,7 @@
         <v>5.4761045470819898</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>45</v>
       </c>
@@ -4969,7 +4953,7 @@
         <v>6.8531803631625161</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>46</v>
       </c>
@@ -4995,7 +4979,7 @@
         <v>5.4143409823497635</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>47</v>
       </c>
@@ -5021,7 +5005,7 @@
         <v>4.4588999947226764</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>48</v>
       </c>
@@ -5047,7 +5031,7 @@
         <v>2.9870121408336701</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>49</v>
       </c>
@@ -5073,7 +5057,7 @@
         <v>4.406740194706229</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>50</v>
       </c>
@@ -5099,7 +5083,7 @@
         <v>4.4098681054030804</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>51</v>
       </c>
@@ -5125,7 +5109,7 @@
         <v>4.9228905915307291</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>52</v>
       </c>
@@ -5151,7 +5135,7 @@
         <v>2.9206667531681152</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>53</v>
       </c>
@@ -5177,7 +5161,7 @@
         <v>4.321656535363438</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>54</v>
       </c>
@@ -5203,7 +5187,7 @@
         <v>4.1465229861948796</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>55</v>
       </c>
@@ -5229,7 +5213,7 @@
         <v>4.549875621324226</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>56</v>
       </c>
@@ -5255,7 +5239,7 @@
         <v>4.9031673830923523</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>57</v>
       </c>
@@ -5281,7 +5265,7 @@
         <v>4.3311154787765931</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>58</v>
       </c>
@@ -5307,7 +5291,7 @@
         <v>4.7381361803980848</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>59</v>
       </c>
@@ -5333,7 +5317,7 @@
         <v>4.2916853495440721</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>60</v>
       </c>
@@ -5359,7 +5343,7 @@
         <v>5.9018451472191913</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>61</v>
       </c>
@@ -5385,7 +5369,7 @@
         <v>4.4682956604673336</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>62</v>
       </c>
@@ -5411,7 +5395,7 @@
         <v>1.3235402196276738</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>63</v>
       </c>
@@ -5437,7 +5421,7 @@
         <v>5.2657210741739036</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>64</v>
       </c>
@@ -5463,7 +5447,7 @@
         <v>6.274190599555884</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>65</v>
       </c>
@@ -5489,7 +5473,7 @@
         <v>2.1300852130325816</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>66</v>
       </c>
@@ -5515,7 +5499,7 @@
         <v>3.9964606398205094</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>67</v>
       </c>
@@ -5541,7 +5525,7 @@
         <v>4.9906169553937563</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>68</v>
       </c>
@@ -5567,7 +5551,7 @@
         <v>3.4083677633622433</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>69</v>
       </c>
@@ -5593,7 +5577,7 @@
         <v>6.4504372893176782</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>70</v>
       </c>
@@ -5619,7 +5603,7 @@
         <v>4.783726724217952</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>71</v>
       </c>
@@ -5645,7 +5629,7 @@
         <v>4.7279922564482151</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>72</v>
       </c>
@@ -5671,7 +5655,7 @@
         <v>3.0663731302319195</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>73</v>
       </c>
@@ -5697,7 +5681,7 @@
         <v>4.0497205948625501</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>74</v>
       </c>
@@ -5723,7 +5707,7 @@
         <v>5.3122689075630243</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>75</v>
       </c>
@@ -5749,7 +5733,7 @@
         <v>6.092073149199142</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>76</v>
       </c>
@@ -5775,7 +5759,7 @@
         <v>5.5246565284178173</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>77</v>
       </c>
@@ -5801,7 +5785,7 @@
         <v>4.4630730338339939</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>78</v>
       </c>
@@ -5827,7 +5811,7 @@
         <v>4.5789133029133025</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>79</v>
       </c>
@@ -5853,7 +5837,7 @@
         <v>5.3514490902051861</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>80</v>
       </c>
@@ -5879,7 +5863,7 @@
         <v>5.4778723896235268</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>81</v>
       </c>
@@ -5905,7 +5889,7 @@
         <v>5.0375993974391164</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>82</v>
       </c>
@@ -5931,7 +5915,7 @@
         <v>4.3950124665035526</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>83</v>
       </c>
@@ -5957,7 +5941,7 @@
         <v>5.4898623028158626</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>89</v>
       </c>
@@ -5983,7 +5967,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>90</v>
       </c>
@@ -6009,7 +5993,7 @@
         <v>6.3250489295576138</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>91</v>
       </c>
@@ -6035,7 +6019,7 @@
         <v>7.6465790557176332</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>92</v>
       </c>
@@ -6061,7 +6045,7 @@
         <v>4.5806588082161621</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>93</v>
       </c>
@@ -6087,7 +6071,7 @@
         <v>6.9242704718318704</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>94</v>
       </c>
@@ -6113,7 +6097,7 @@
         <v>7.3170989500569483</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>95</v>
       </c>
@@ -6139,7 +6123,7 @@
         <v>7.1643186920438833</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>96</v>
       </c>
@@ -6165,7 +6149,7 @@
         <v>6.002998612380277</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>97</v>
       </c>
@@ -6191,7 +6175,7 @@
         <v>6.6389581341445769</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>255</v>
       </c>
@@ -6217,7 +6201,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>256</v>
       </c>
@@ -6243,7 +6227,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>257</v>
       </c>
@@ -6269,7 +6253,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>258</v>
       </c>
@@ -6295,7 +6279,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>259</v>
       </c>
@@ -6321,7 +6305,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>260</v>
       </c>
@@ -6347,7 +6331,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>261</v>
       </c>
@@ -6373,7 +6357,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>262</v>
       </c>
@@ -6399,7 +6383,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>263</v>
       </c>
@@ -6425,7 +6409,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>264</v>
       </c>
@@ -6451,7 +6435,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>265</v>
       </c>
@@ -6477,7 +6461,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>266</v>
       </c>
@@ -6503,7 +6487,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>267</v>
       </c>
@@ -6529,7 +6513,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>268</v>
       </c>
@@ -6555,7 +6539,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>115</v>
       </c>
@@ -6581,7 +6565,7 @@
         <v>6.89</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>116</v>
       </c>
@@ -6607,7 +6591,7 @@
         <v>4.3057219698533959</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>117</v>
       </c>
@@ -6633,7 +6617,7 @@
         <v>4.4186763570297538</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>118</v>
       </c>
@@ -6659,7 +6643,7 @@
         <v>6.2103254317323993</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>119</v>
       </c>
@@ -6685,7 +6669,7 @@
         <v>9.9636002885039083</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>120</v>
       </c>
@@ -6711,7 +6695,7 @@
         <v>6.0816611128526628</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>121</v>
       </c>
@@ -6737,7 +6721,7 @@
         <v>4.2475948540300399</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>122</v>
       </c>
@@ -6763,7 +6747,7 @@
         <v>7.0147055437058095</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>123</v>
       </c>
@@ -6789,7 +6773,7 @@
         <v>4.1193297356525456</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>124</v>
       </c>
@@ -6815,7 +6799,7 @@
         <v>5.1085265888479849</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>125</v>
       </c>
@@ -6841,7 +6825,7 @@
         <v>7.1295120056900352</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>126</v>
       </c>
@@ -6867,7 +6851,7 @@
         <v>7.0265904589934758</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>127</v>
       </c>
@@ -6893,7 +6877,7 @@
         <v>6.7174189184485167</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>128</v>
       </c>
@@ -6919,7 +6903,7 @@
         <v>6.8637733588374203</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>129</v>
       </c>
@@ -6945,7 +6929,7 @@
         <v>4.823199080142893</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>130</v>
       </c>
@@ -6971,7 +6955,7 @@
         <v>8.8147920530959158</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>131</v>
       </c>
@@ -6997,7 +6981,7 @@
         <v>7.9774148072271922</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>132</v>
       </c>
@@ -7023,7 +7007,7 @@
         <v>6.068034704614603</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>133</v>
       </c>
@@ -7049,7 +7033,7 @@
         <v>5.7484637378150891</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>134</v>
       </c>
@@ -7075,7 +7059,7 @@
         <v>5.1790080818965496</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>135</v>
       </c>
@@ -7101,7 +7085,7 @@
         <v>5.4623828288082947</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>136</v>
       </c>
@@ -7127,7 +7111,7 @@
         <v>5.0679748867069474</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>137</v>
       </c>
@@ -7153,7 +7137,7 @@
         <v>4.7373153118609395</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>138</v>
       </c>
@@ -7179,7 +7163,7 @@
         <v>5.2500742551910919</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>139</v>
       </c>
@@ -7205,7 +7189,7 @@
         <v>6.5145176640120557</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>140</v>
       </c>
@@ -7231,7 +7215,7 @@
         <v>4.88727931703494</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>141</v>
       </c>
@@ -7257,7 +7241,7 @@
         <v>7.4244235712930005</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>153</v>
       </c>
@@ -7283,7 +7267,7 @@
         <v>4.3045005423875899</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>154</v>
       </c>
@@ -7309,7 +7293,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>155</v>
       </c>
@@ -7335,7 +7319,7 @@
         <v>4.72</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>156</v>
       </c>
@@ -7361,7 +7345,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>157</v>
       </c>
@@ -7387,7 +7371,7 @@
         <v>4.84</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>158</v>
       </c>
@@ -7413,7 +7397,7 @@
         <v>5.05</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>159</v>
       </c>
@@ -7439,7 +7423,7 @@
         <v>4.8099999999999996</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>160</v>
       </c>
@@ -7465,7 +7449,7 @@
         <v>4.5599999999999996</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>161</v>
       </c>
@@ -7491,7 +7475,7 @@
         <v>3.08</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>162</v>
       </c>
@@ -7517,7 +7501,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>163</v>
       </c>
@@ -7543,7 +7527,7 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>164</v>
       </c>
@@ -7569,7 +7553,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>165</v>
       </c>
@@ -7595,7 +7579,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>166</v>
       </c>
@@ -7621,7 +7605,7 @@
         <v>4.78</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>167</v>
       </c>
@@ -7647,7 +7631,7 @@
         <v>4.5599999999999996</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>168</v>
       </c>
@@ -7673,7 +7657,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>169</v>
       </c>
@@ -7699,7 +7683,7 @@
         <v>3.86</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>170</v>
       </c>
@@ -7725,7 +7709,7 @@
         <v>4.37</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>171</v>
       </c>
@@ -7751,7 +7735,7 @@
         <v>5.38</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>172</v>
       </c>
@@ -7777,7 +7761,7 @@
         <v>3.34</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>173</v>
       </c>
@@ -7803,7 +7787,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>174</v>
       </c>
@@ -7829,7 +7813,7 @@
         <v>4.51</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>98</v>
       </c>
@@ -7855,7 +7839,7 @@
         <v>3.479979931723296</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>99</v>
       </c>
@@ -7881,7 +7865,7 @@
         <v>6.0143320558947666</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>100</v>
       </c>
@@ -7907,7 +7891,7 @@
         <v>3.8034085146560166</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>101</v>
       </c>
@@ -7933,7 +7917,7 @@
         <v>3.9790535299442027</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>102</v>
       </c>
@@ -7959,7 +7943,7 @@
         <v>3.1221585283251221</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>103</v>
       </c>
@@ -7985,7 +7969,7 @@
         <v>6.1909360342241602</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>104</v>
       </c>
@@ -8011,7 +7995,7 @@
         <v>5.7033366474327964</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>105</v>
       </c>
@@ -8037,7 +8021,7 @@
         <v>6.8059632228139142</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>106</v>
       </c>
@@ -8063,7 +8047,7 @@
         <v>4.7485803033179561</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>107</v>
       </c>
@@ -8089,7 +8073,7 @@
         <v>4.5801556036460873</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>108</v>
       </c>
@@ -8115,7 +8099,7 @@
         <v>4.8525783477926634</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>109</v>
       </c>
@@ -8141,7 +8125,7 @@
         <v>5.2142839622383717</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>110</v>
       </c>
@@ -8167,7 +8151,7 @@
         <v>2.6176170107085124</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>111</v>
       </c>
@@ -8193,7 +8177,7 @@
         <v>5.2013415810924188</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>112</v>
       </c>
@@ -8219,7 +8203,7 @@
         <v>5.8299986631176068</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>113</v>
       </c>
@@ -8245,7 +8229,7 @@
         <v>7.9500863459915045</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>114</v>
       </c>
@@ -8271,7 +8255,7 @@
         <v>6.5444998134751993</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>142</v>
       </c>
@@ -8297,7 +8281,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>143</v>
       </c>
@@ -8323,7 +8307,7 @@
         <v>4.4960228331652345</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>144</v>
       </c>
@@ -8349,7 +8333,7 @@
         <v>3.0208054837847547</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>145</v>
       </c>
@@ -8375,7 +8359,7 @@
         <v>5.2468514295737592</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>146</v>
       </c>
@@ -8401,7 +8385,7 @@
         <v>5.4250332074965693</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>147</v>
       </c>
@@ -8427,7 +8411,7 @@
         <v>8.5405129248000797</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>148</v>
       </c>
@@ -8453,7 +8437,7 @@
         <v>7.3509825140531841</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>149</v>
       </c>
@@ -8479,7 +8463,7 @@
         <v>8.0306707900215848</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>150</v>
       </c>
@@ -8505,7 +8489,7 @@
         <v>9.6740922645149983</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>151</v>
       </c>
@@ -8531,7 +8515,7 @@
         <v>8.1269087276761773</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>152</v>
       </c>
@@ -8557,7 +8541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>273</v>
       </c>
@@ -8583,7 +8567,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>274</v>
       </c>
@@ -8609,7 +8593,7 @@
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>275</v>
       </c>
@@ -8635,7 +8619,7 @@
         <v>5.65</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>276</v>
       </c>
@@ -8661,7 +8645,7 @@
         <v>10.89</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>277</v>
       </c>
@@ -8687,7 +8671,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>278</v>
       </c>
@@ -8713,7 +8697,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>279</v>
       </c>
@@ -8739,7 +8723,7 @@
         <v>11.26</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>280</v>
       </c>
@@ -8765,7 +8749,7 @@
         <v>9.7799999999999994</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>281</v>
       </c>
@@ -8791,7 +8775,7 @@
         <v>11.92</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>282</v>
       </c>
@@ -8817,7 +8801,7 @@
         <v>7.18</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>283</v>
       </c>
@@ -8836,14 +8820,14 @@
       <c r="F275" s="2">
         <v>94</v>
       </c>
-      <c r="G275" s="4">
+      <c r="G275" s="6">
         <v>0</v>
       </c>
       <c r="H275" s="3">
         <v>9.5500000000000007</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>284</v>
       </c>
@@ -8869,7 +8853,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>285</v>
       </c>
@@ -8895,7 +8879,7 @@
         <v>14.52</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>286</v>
       </c>
@@ -8921,7 +8905,7 @@
         <v>16.907663855493748</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>287</v>
       </c>
@@ -8947,7 +8931,7 @@
         <v>17.946369038698293</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>288</v>
       </c>
@@ -8973,7 +8957,7 @@
         <v>6.74</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>289</v>
       </c>
@@ -8999,7 +8983,7 @@
         <v>10.15</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>290</v>
       </c>
@@ -9025,7 +9009,7 @@
         <v>7.18</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>291</v>
       </c>
@@ -9051,7 +9035,7 @@
         <v>13.63</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>292</v>
       </c>
@@ -9077,7 +9061,7 @@
         <v>6.29</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>293</v>
       </c>
@@ -9103,7 +9087,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>294</v>
       </c>
@@ -9129,7 +9113,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>295</v>
       </c>
@@ -9155,7 +9139,7 @@
         <v>7.04</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>296</v>
       </c>
@@ -9171,13 +9155,13 @@
       <c r="E288" s="3">
         <v>0.75294117647058822</v>
       </c>
-      <c r="F288" s="5"/>
-      <c r="G288" s="6"/>
+      <c r="F288" s="4"/>
+      <c r="G288" s="5"/>
       <c r="H288" s="3">
         <v>9.48</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>297</v>
       </c>
@@ -9203,7 +9187,7 @@
         <v>9.85</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>298</v>
       </c>
@@ -9229,7 +9213,7 @@
         <v>13.26</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>299</v>
       </c>
@@ -9255,7 +9239,7 @@
         <v>4.96</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>300</v>
       </c>
@@ -9281,7 +9265,7 @@
         <v>14.15</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>301</v>
       </c>
@@ -9307,7 +9291,7 @@
         <v>9.92</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>302</v>
       </c>
@@ -9333,7 +9317,7 @@
         <v>16.525067319301684</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>303</v>
       </c>
@@ -9359,7 +9343,7 @@
         <v>11.872526842380347</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>304</v>
       </c>
@@ -9385,7 +9369,7 @@
         <v>9.9257384044098984</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>305</v>
       </c>
@@ -9409,7 +9393,7 @@
         <v>4.653626630101817</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>306</v>
       </c>
@@ -9435,7 +9419,7 @@
         <v>13.779506973513442</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>307</v>
       </c>
@@ -9461,7 +9445,7 @@
         <v>13.578995161462288</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>308</v>
       </c>
@@ -9487,7 +9471,7 @@
         <v>11.970784907420295</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>309</v>
       </c>
@@ -9513,7 +9497,7 @@
         <v>13.420515069503434</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
         <v>310</v>
       </c>
@@ -9539,7 +9523,7 @@
         <v>11.633260843525827</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
         <v>311</v>
       </c>
@@ -9565,7 +9549,7 @@
         <v>10.069696812645763</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>312</v>
       </c>
@@ -9591,7 +9575,7 @@
         <v>4.899704364100482</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>313</v>
       </c>
@@ -9617,7 +9601,7 @@
         <v>10.580640748332444</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
         <v>314</v>
       </c>
@@ -9643,7 +9627,7 @@
         <v>20.151058869510802</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
         <v>315</v>
       </c>
@@ -9669,7 +9653,7 @@
         <v>8.2216296881057271</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
         <v>316</v>
       </c>
@@ -9695,7 +9679,7 @@
         <v>12.131932980664665</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
         <v>317</v>
       </c>
@@ -9717,7 +9701,7 @@
         <v>21.87158094945444</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
         <v>318</v>
       </c>
@@ -9743,7 +9727,7 @@
         <v>11.380744839199533</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
         <v>319</v>
       </c>
@@ -9764,7 +9748,7 @@
         <v>6.7191700303930615</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
         <v>320</v>
       </c>
@@ -9790,7 +9774,7 @@
         <v>13.322967400881058</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
         <v>321</v>
       </c>
@@ -9816,7 +9800,7 @@
         <v>9.3749665603966221</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
         <v>322</v>
       </c>
@@ -9842,7 +9826,7 @@
         <v>18.763487621765837</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
         <v>323</v>
       </c>
@@ -9868,7 +9852,7 @@
         <v>9.7875218594999556</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
         <v>324</v>
       </c>
@@ -9894,7 +9878,7 @@
         <v>9.7766311748689247</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
         <v>325</v>
       </c>
@@ -9920,7 +9904,7 @@
         <v>2.3254577769412039</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
         <v>326</v>
       </c>
@@ -9946,7 +9930,7 @@
         <v>5.1132021808650858</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
         <v>327</v>
       </c>
@@ -9972,7 +9956,7 @@
         <v>6.4433495215595835</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
         <v>328</v>
       </c>
@@ -9998,7 +9982,7 @@
         <v>6.9428995907917939</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
         <v>329</v>
       </c>
@@ -10024,7 +10008,7 @@
         <v>7.1643021562717379</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
         <v>330</v>
       </c>
@@ -10050,7 +10034,7 @@
         <v>4.9572291373926181</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
         <v>331</v>
       </c>
@@ -10073,7 +10057,7 @@
         <v>4.1554692627037229</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
         <v>332</v>
       </c>
@@ -10099,7 +10083,7 @@
         <v>2.9493783571967924</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>333</v>
       </c>
@@ -10125,7 +10109,7 @@
         <v>3.5241110352634899</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
         <v>334</v>
       </c>
@@ -10151,7 +10135,7 @@
         <v>5.716960447160246</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
         <v>335</v>
       </c>
@@ -10177,7 +10161,7 @@
         <v>5.2912860047441539</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
         <v>336</v>
       </c>
@@ -10203,7 +10187,7 @@
         <v>3.3848144632043482</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
         <v>337</v>
       </c>
@@ -10229,7 +10213,7 @@
         <v>5.1092500756437422</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
         <v>338</v>
       </c>
@@ -10255,7 +10239,7 @@
         <v>3.0285177677734132</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
         <v>339</v>
       </c>
@@ -10281,7 +10265,7 @@
         <v>2.480352422907488</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
         <v>340</v>
       </c>
@@ -10307,7 +10291,7 @@
         <v>5.6852365311872486</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
         <v>341</v>
       </c>
@@ -10333,7 +10317,7 @@
         <v>7.92</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
         <v>342</v>
       </c>
@@ -10359,7 +10343,7 @@
         <v>4.8899999999999997</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
         <v>343</v>
       </c>
@@ -10385,7 +10369,7 @@
         <v>5.1100000000000003</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
         <v>344</v>
       </c>
@@ -10411,7 +10395,7 @@
         <v>5.33</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
         <v>345</v>
       </c>
@@ -10437,7 +10421,7 @@
         <v>3.78</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
         <v>346</v>
       </c>
@@ -10463,7 +10447,7 @@
         <v>5.65</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
         <v>347</v>
       </c>
@@ -10489,7 +10473,7 @@
         <v>5.78</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
         <v>348</v>
       </c>
@@ -10515,7 +10499,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
         <v>349</v>
       </c>
@@ -10541,7 +10525,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
         <v>350</v>
       </c>
@@ -10567,7 +10551,7 @@
         <v>3.78</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
         <v>351</v>
       </c>
@@ -10593,7 +10577,7 @@
         <v>6.15</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
         <v>352</v>
       </c>
@@ -10619,7 +10603,7 @@
         <v>4.07</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
         <v>353</v>
       </c>
@@ -10643,7 +10627,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
         <v>354</v>
       </c>
@@ -10669,7 +10653,7 @@
         <v>3.78</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
         <v>355</v>
       </c>
@@ -10695,7 +10679,7 @@
         <v>3.78</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
         <v>356</v>
       </c>
@@ -10721,7 +10705,7 @@
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
         <v>357</v>
       </c>
@@ -10747,7 +10731,7 @@
         <v>7.18</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
         <v>358</v>
       </c>
@@ -10773,7 +10757,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
         <v>359</v>
       </c>
@@ -10799,7 +10783,7 @@
         <v>5.04</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
         <v>360</v>
       </c>
@@ -10825,7 +10809,7 @@
         <v>4.59</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
         <v>361</v>
       </c>
@@ -10851,7 +10835,7 @@
         <v>0.74402787791177094</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
         <v>362</v>
       </c>
@@ -10875,7 +10859,7 @@
         <v>2.8083668550638845</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
         <v>363</v>
       </c>
@@ -10901,7 +10885,7 @@
         <v>4.7987100851299775</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
         <v>364</v>
       </c>
@@ -10927,7 +10911,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
         <v>365</v>
       </c>
@@ -10953,7 +10937,7 @@
         <v>2.7366522241034317</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
         <v>366</v>
       </c>
@@ -10979,7 +10963,7 @@
         <v>5.04</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
         <v>367</v>
       </c>
@@ -11005,7 +10989,7 @@
         <v>4.74</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
         <v>368</v>
       </c>
@@ -11031,7 +11015,7 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
         <v>369</v>
       </c>
@@ -11057,7 +11041,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
         <v>370</v>
       </c>
@@ -11083,7 +11067,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
         <v>371</v>
       </c>
@@ -11109,7 +11093,7 @@
         <v>6.29</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
         <v>372</v>
       </c>
@@ -11135,7 +11119,7 @@
         <v>5.33</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
         <v>373</v>
       </c>
@@ -11161,7 +11145,7 @@
         <v>5.48</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
         <v>374</v>
       </c>
@@ -11187,7 +11171,7 @@
         <v>6.22</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
         <v>375</v>
       </c>
@@ -11211,7 +11195,7 @@
         <v>3.4621986801919715</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
         <v>376</v>
       </c>
@@ -11237,7 +11221,7 @@
         <v>9.11</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
         <v>377</v>
       </c>
@@ -11263,7 +11247,7 @@
         <v>3.195063771995434</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
         <v>378</v>
       </c>
@@ -11289,7 +11273,7 @@
         <v>0.3684584589593784</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
         <v>379</v>
       </c>
@@ -11313,7 +11297,7 @@
         <v>3.56</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
         <v>380</v>
       </c>
@@ -11339,7 +11323,7 @@
         <v>7.11</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
         <v>381</v>
       </c>
@@ -11365,7 +11349,7 @@
         <v>5.4688856378583832</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
         <v>382</v>
       </c>
@@ -11391,7 +11375,7 @@
         <v>5.9374036690339098</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
         <v>383</v>
       </c>
@@ -11417,7 +11401,7 @@
         <v>6.3275885086732577</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
         <v>384</v>
       </c>
@@ -11443,7 +11427,7 @@
         <v>6.1973316319766667</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
         <v>385</v>
       </c>
@@ -11469,7 +11453,7 @@
         <v>5.3883503785191955</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
         <v>386</v>
       </c>
@@ -11495,7 +11479,7 @@
         <v>5.9755531898320031</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
         <v>387</v>
       </c>
@@ -11521,7 +11505,7 @@
         <v>6.3164765983155045</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
         <v>388</v>
       </c>
@@ -11545,7 +11529,7 @@
         <v>6.8280182870425268</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
         <v>389</v>
       </c>
@@ -11571,7 +11555,7 @@
         <v>5.1242240854366523</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
         <v>390</v>
       </c>
@@ -11597,7 +11581,7 @@
         <v>5.6918084132245772</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
         <v>391</v>
       </c>
@@ -11623,7 +11607,7 @@
         <v>5.8489476163171679</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
         <v>392</v>
       </c>
@@ -11649,7 +11633,7 @@
         <v>8.6292958546392118</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
         <v>393</v>
       </c>
@@ -11675,7 +11659,7 @@
         <v>3.4056266763399723</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
         <v>394</v>
       </c>
@@ -11701,7 +11685,7 @@
         <v>5.3522705115749272</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
         <v>395</v>
       </c>
@@ -11727,7 +11711,7 @@
         <v>5.7798312285568292</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
         <v>396</v>
       </c>
@@ -11753,7 +11737,7 @@
         <v>7.9357451664876475</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
         <v>397</v>
       </c>
@@ -11779,7 +11763,7 @@
         <v>4.2255176402544823</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
         <v>398</v>
       </c>
@@ -11805,7 +11789,7 @@
         <v>5.9259957049792771</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
         <v>399</v>
       </c>
@@ -11831,7 +11815,7 @@
         <v>2.6901630001203363</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
         <v>400</v>
       </c>
@@ -11857,7 +11841,7 @@
         <v>5.3376598616386337</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
         <v>401</v>
       </c>
@@ -11883,7 +11867,7 @@
         <v>5.0469236150334487</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
         <v>402</v>
       </c>
@@ -11909,7 +11893,7 @@
         <v>5.6322974101921481</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
         <v>403</v>
       </c>
@@ -11935,7 +11919,7 @@
         <v>6.0295423670096753</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
         <v>404</v>
       </c>
@@ -11961,7 +11945,7 @@
         <v>4.7952192607266673</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
         <v>405</v>
       </c>
@@ -11987,7 +11971,7 @@
         <v>6.2919533713315543</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
         <v>406</v>
       </c>
@@ -12013,7 +11997,7 @@
         <v>5.5254973954809907</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
         <v>407</v>
       </c>
@@ -12039,7 +12023,7 @@
         <v>6.1232968090959101</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
         <v>408</v>
       </c>
@@ -12065,7 +12049,7 @@
         <v>5.0070350856445742</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
         <v>409</v>
       </c>
@@ -12073,8 +12057,8 @@
         <v>3</v>
       </c>
       <c r="C401" s="2" cm="1">
-        <f t="array" aca="1" ref="C401" ca="1">C3:C40117</f>
-        <v>0</v>
+        <f t="array" ref="C401">C3:C40117</f>
+        <v>7</v>
       </c>
       <c r="D401" s="3">
         <v>15.450469750806533</v>

</xml_diff>